<commit_message>
Added Row Reader and Brainstormed the Algorithm
Feel free to delete what's there of the latter. I wouldn't recommend deleting the former.
</commit_message>
<xml_diff>
--- a/CS2033template.xlsx
+++ b/CS2033template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jddju\eclipse-workspace\Project\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC50C3C-6EFA-4ECF-9047-47B62C30D801}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18432" windowHeight="1656" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="2745"/>
   </bookViews>
   <sheets>
     <sheet name="Week" sheetId="1" r:id="rId1"/>
@@ -20,6 +14,7 @@
     <sheet name="TalleySheet" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:U7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nicholas</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{A140FCF5-02B0-407D-AA26-535831E58569}">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{E3B44143-EE11-413D-83E5-0768840A01F0}">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -87,12 +82,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nicholas</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -145,12 +140,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nicholas</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -304,7 +299,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -645,20 +640,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="31" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -705,7 +700,7 @@
       <c r="AD1" s="2"/>
       <c r="AE1" s="2"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -713,22 +708,22 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
       <c r="F2" t="s">
         <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -739,10 +734,10 @@
         <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
         <v>39</v>
@@ -751,7 +746,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -774,27 +769,27 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -809,20 +804,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="31" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -845,7 +840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -880,17 +875,17 @@
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -903,21 +898,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -943,7 +938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -969,7 +964,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -995,7 +990,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1021,7 +1016,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1054,19 +1049,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1077,7 +1072,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1089,12 +1084,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Supply Reader - FULLY FUNCTIONAL
</commit_message>
<xml_diff>
--- a/CS2033template.xlsx
+++ b/CS2033template.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D733E83F-3403-4376-A57A-D4E46DCB2311}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="2745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16605" windowHeight="1605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
     <sheet name="TalleySheet" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:U7"/>
+  <oleSize ref="A1:R8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nicholas</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -82,12 +83,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nicholas</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -111,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -140,12 +141,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nicholas</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -174,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -218,9 +219,6 @@
     <t>SCI4311</t>
   </si>
   <si>
-    <t>Free</t>
-  </si>
-  <si>
     <t>MATH321</t>
   </si>
   <si>
@@ -293,13 +291,13 @@
     <t>ENGL1719</t>
   </si>
   <si>
-    <t>I</t>
+    <t>P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -640,11 +638,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,94 +700,94 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C3">
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="D4">
+        <v>123</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -804,7 +802,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -842,7 +840,7 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -877,17 +875,17 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -898,11 +896,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,7 +938,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -955,91 +953,91 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>37</v>
       </c>
-      <c r="F5" t="s">
-        <v>38</v>
-      </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1049,7 +1047,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1074,7 +1072,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1084,7 +1082,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>